<commit_message>
Updateing Test Case data
</commit_message>
<xml_diff>
--- a/src/main/java/testData/Test Cases Data.xlsx
+++ b/src/main/java/testData/Test Cases Data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>Description</t>
   </si>
@@ -32,9 +32,6 @@
     <t>BrowserType</t>
   </si>
   <si>
-    <t>IE</t>
-  </si>
-  <si>
     <t>Url</t>
   </si>
   <si>
@@ -77,17 +74,13 @@
     <t>n</t>
   </si>
   <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Skip</t>
+    <t>FF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -551,21 +544,21 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="17.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="9.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="13.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="28.42578125" collapsed="true"/>
-    <col min="5" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="17.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="28.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -573,13 +566,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>0</v>
@@ -587,24 +580,22 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="2"/>
@@ -631,75 +622,75 @@
   <dimension ref="A1:AS4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="4" width="9.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="13.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="12.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="4" width="31.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="4" width="22.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="4" width="16.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="4" width="16.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="4" width="19.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="4" width="13.85546875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="4" width="39.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="4" width="35.42578125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="4" width="17.0" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="4" width="19.42578125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="4" width="18.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="4" width="18.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="4" width="18.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="4" width="21.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="4" width="18.140625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="4" width="21.140625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="4" width="18.85546875" collapsed="true"/>
-    <col min="21" max="22" bestFit="true" customWidth="true" style="4" width="16.5703125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="4" width="12.5703125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="4" width="8.140625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="4" width="25.5703125" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="4" width="35.5703125" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="4" width="47.0" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="4" width="33.42578125" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="4" width="20.85546875" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="4" width="8.42578125" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="4" width="9.7109375" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="4" width="8.85546875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="4" width="16.5703125" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="4" width="37.140625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="4" width="9.28515625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" style="4" width="18.140625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" style="4" width="24.5703125" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" style="4" width="21.42578125" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" style="4" width="23.140625" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" style="4" width="12.85546875" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" style="4" width="18.0" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" style="4" width="14.85546875" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" style="4" width="21.0" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" style="4" width="25.85546875" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" style="4" width="16.42578125" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" style="4" width="15.28515625" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" style="4" width="18.5703125" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" style="4" width="19.85546875" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" style="4" width="11.0" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" style="4" width="19.5703125" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" style="4" width="14.85546875" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" style="4" width="21.0" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" style="4" width="25.85546875" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" style="4" width="16.42578125" collapsed="true"/>
-    <col min="55" max="55" bestFit="true" customWidth="true" style="4" width="15.28515625" collapsed="true"/>
-    <col min="56" max="56" bestFit="true" customWidth="true" style="4" width="18.5703125" collapsed="true"/>
-    <col min="57" max="57" bestFit="true" customWidth="true" style="4" width="19.85546875" collapsed="true"/>
-    <col min="58" max="58" bestFit="true" customWidth="true" style="4" width="11.0" collapsed="true"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" style="4" width="19.5703125" collapsed="true"/>
-    <col min="60" max="16384" style="4" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="39.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="35.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="19.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="18.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="18.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="21.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="18.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="21.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="18.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="22" width="16.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="8.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="25.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="35.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="47" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="33.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="20.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="8.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="9.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="16.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="37.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="9.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="18.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="24.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="21.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="23.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="12.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="18" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="14.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="21" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="25.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="16.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="15.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="18.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="19.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="11" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="19.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="14.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="21" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="25.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="16.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="15.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="18.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="19.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="11" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="19.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="16384" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -751,13 +742,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>2</v>
@@ -807,22 +798,20 @@
     </row>
     <row r="3" spans="1:45" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>20</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>15</v>
-      </c>
       <c r="F3" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -866,22 +855,20 @@
     </row>
     <row r="4" spans="1:45" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="D4" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>

</xml_diff>